<commit_message>
Adding back abstract promptType for media intents.
</commit_message>
<xml_diff>
--- a/form-files/IMNCI/breakdowns.xlsx
+++ b/form-files/IMNCI/breakdowns.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="693" count="1083">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="692" count="1083">
   <si>
     <t>comments</t>
   </si>
@@ -1317,9 +1317,6 @@
   </si>
   <si>
     <t>दिन मैं कितनी बार?</t>
-  </si>
-  <si>
-    <t>number</t>
   </si>
   <si>
     <t>serving_size</t>
@@ -5126,31 +5123,31 @@
     <row r="233">
       <c s="12" r="A233"/>
       <c t="s" r="B233">
-        <v>425</v>
+        <v>24</v>
       </c>
       <c t="s" r="C233">
         <v>422</v>
       </c>
       <c t="s" r="D233">
+        <v>425</v>
+      </c>
+      <c t="s" r="F233">
         <v>426</v>
       </c>
-      <c t="s" r="F233">
+      <c t="s" r="G233">
         <v>427</v>
-      </c>
-      <c t="s" r="G233">
-        <v>428</v>
       </c>
     </row>
     <row r="234">
       <c s="12" r="A234"/>
       <c t="s" r="B234">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c t="s" r="C234">
         <v>422</v>
       </c>
       <c t="s" r="D234">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="235">
@@ -5162,33 +5159,33 @@
         <v>422</v>
       </c>
       <c t="s" r="D235">
+        <v>430</v>
+      </c>
+      <c t="s" r="F235">
         <v>431</v>
       </c>
-      <c t="s" r="F235">
+      <c t="s" r="G235">
         <v>432</v>
-      </c>
-      <c t="s" r="G235">
-        <v>433</v>
       </c>
     </row>
     <row r="236">
       <c t="s" s="12" r="A236">
+        <v>433</v>
+      </c>
+      <c t="s" r="B236">
         <v>434</v>
-      </c>
-      <c t="s" r="B236">
-        <v>435</v>
       </c>
       <c t="s" r="C236">
         <v>422</v>
       </c>
       <c t="s" r="D236">
+        <v>435</v>
+      </c>
+      <c t="s" r="F236">
         <v>436</v>
       </c>
-      <c t="s" r="F236">
+      <c t="s" r="G236">
         <v>437</v>
-      </c>
-      <c t="s" r="G236">
-        <v>438</v>
       </c>
     </row>
     <row r="237">
@@ -5209,33 +5206,33 @@
         <v>90</v>
       </c>
       <c t="s" r="D239">
+        <v>438</v>
+      </c>
+      <c t="s" r="F239">
         <v>439</v>
       </c>
-      <c t="s" r="F239">
+      <c t="s" r="G239">
         <v>440</v>
-      </c>
-      <c t="s" r="G239">
-        <v>441</v>
       </c>
     </row>
     <row r="240">
       <c t="s" s="12" r="A240">
+        <v>441</v>
+      </c>
+      <c t="s" r="B240">
+        <v>434</v>
+      </c>
+      <c t="s" r="C240">
         <v>442</v>
       </c>
-      <c t="s" r="B240">
-        <v>435</v>
-      </c>
-      <c t="s" r="C240">
+      <c t="s" r="D240">
         <v>443</v>
       </c>
-      <c t="s" r="D240">
+      <c t="s" r="F240">
         <v>444</v>
       </c>
-      <c t="s" r="F240">
+      <c t="s" r="G240">
         <v>445</v>
-      </c>
-      <c t="s" r="G240">
-        <v>446</v>
       </c>
     </row>
     <row r="241">
@@ -5247,7 +5244,7 @@
     <row r="242">
       <c s="12" r="A242"/>
       <c t="s" r="B242">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c t="s" r="C242">
         <v>359</v>
@@ -5256,31 +5253,31 @@
     <row r="243">
       <c s="12" r="A243"/>
       <c t="s" r="B243">
+        <v>447</v>
+      </c>
+      <c t="s" r="C243">
         <v>448</v>
-      </c>
-      <c t="s" r="C243">
-        <v>449</v>
       </c>
     </row>
     <row r="244">
       <c s="12" r="A244"/>
       <c t="s" r="B244">
+        <v>449</v>
+      </c>
+      <c t="s" r="C244">
         <v>450</v>
-      </c>
-      <c t="s" r="C244">
-        <v>451</v>
       </c>
     </row>
     <row r="245">
       <c s="12" r="A245"/>
       <c t="s" r="B245">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="246">
       <c s="12" r="A246"/>
       <c t="s" s="8" r="B246">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="247">
@@ -5295,10 +5292,10 @@
         <v>30</v>
       </c>
       <c t="s" r="F248">
+        <v>453</v>
+      </c>
+      <c t="s" r="G248">
         <v>454</v>
-      </c>
-      <c t="s" r="G248">
-        <v>455</v>
       </c>
     </row>
     <row r="249">
@@ -5307,13 +5304,13 @@
         <v>30</v>
       </c>
       <c t="s" r="C249">
+        <v>455</v>
+      </c>
+      <c t="s" r="F249">
         <v>456</v>
       </c>
-      <c t="s" r="F249">
+      <c t="s" r="G249">
         <v>457</v>
-      </c>
-      <c t="s" r="G249">
-        <v>458</v>
       </c>
     </row>
     <row r="250">
@@ -5322,13 +5319,13 @@
         <v>30</v>
       </c>
       <c t="s" r="C250">
+        <v>458</v>
+      </c>
+      <c t="s" r="F250">
         <v>459</v>
       </c>
-      <c t="s" r="F250">
+      <c t="s" r="G250">
         <v>460</v>
-      </c>
-      <c t="s" r="G250">
-        <v>461</v>
       </c>
     </row>
     <row r="251">
@@ -5337,13 +5334,13 @@
         <v>30</v>
       </c>
       <c t="s" r="C251">
+        <v>461</v>
+      </c>
+      <c t="s" r="F251">
         <v>462</v>
       </c>
-      <c t="s" r="F251">
+      <c t="s" r="G251">
         <v>463</v>
-      </c>
-      <c t="s" r="G251">
-        <v>464</v>
       </c>
     </row>
     <row r="252">
@@ -5364,10 +5361,10 @@
         <v>30</v>
       </c>
       <c t="s" r="F254">
+        <v>464</v>
+      </c>
+      <c t="s" r="G254">
         <v>465</v>
-      </c>
-      <c t="s" r="G254">
-        <v>466</v>
       </c>
     </row>
     <row r="255">
@@ -5376,7 +5373,7 @@
         <v>30</v>
       </c>
       <c t="s" r="F255">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c s="9" r="G255"/>
     </row>
@@ -5386,13 +5383,13 @@
         <v>30</v>
       </c>
       <c t="s" r="C256">
+        <v>467</v>
+      </c>
+      <c t="s" r="F256">
         <v>468</v>
       </c>
-      <c t="s" r="F256">
-        <v>469</v>
-      </c>
       <c t="s" r="G256">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="257">
@@ -5401,13 +5398,13 @@
         <v>30</v>
       </c>
       <c t="s" r="C257">
+        <v>469</v>
+      </c>
+      <c t="s" r="F257">
         <v>470</v>
       </c>
-      <c t="s" r="F257">
-        <v>471</v>
-      </c>
       <c t="s" r="G257">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="258">
@@ -5422,33 +5419,33 @@
         <v>30</v>
       </c>
       <c t="s" r="F259">
+        <v>471</v>
+      </c>
+      <c t="s" r="G259">
         <v>472</v>
       </c>
-      <c t="s" r="G259">
+      <c t="s" r="H259">
         <v>473</v>
       </c>
-      <c t="s" r="H259">
+      <c t="s" r="I259">
         <v>474</v>
-      </c>
-      <c t="s" r="I259">
-        <v>475</v>
       </c>
     </row>
     <row r="260">
       <c s="12" r="A260"/>
       <c t="s" r="B260">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="261">
       <c s="12" r="A261"/>
       <c t="s" s="8" r="B261">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="262">
       <c t="s" s="12" r="A262">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c t="s" r="B262">
         <v>29</v>
@@ -5463,10 +5460,10 @@
         <v>30</v>
       </c>
       <c t="s" r="F263">
+        <v>453</v>
+      </c>
+      <c t="s" r="G263">
         <v>454</v>
-      </c>
-      <c t="s" r="G263">
-        <v>455</v>
       </c>
     </row>
     <row r="264">
@@ -5477,7 +5474,7 @@
     </row>
     <row r="265">
       <c t="s" s="12" r="A265">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c t="s" r="B265">
         <v>29</v>
@@ -5492,10 +5489,10 @@
         <v>30</v>
       </c>
       <c t="s" r="F266">
+        <v>464</v>
+      </c>
+      <c t="s" r="G266">
         <v>465</v>
-      </c>
-      <c t="s" r="G266">
-        <v>466</v>
       </c>
     </row>
     <row r="267">
@@ -5516,10 +5513,10 @@
         <v>30</v>
       </c>
       <c t="s" r="F269">
+        <v>478</v>
+      </c>
+      <c t="s" r="G269">
         <v>479</v>
-      </c>
-      <c t="s" r="G269">
-        <v>480</v>
       </c>
     </row>
     <row r="270">
@@ -5528,10 +5525,10 @@
         <v>30</v>
       </c>
       <c t="s" r="F270">
+        <v>480</v>
+      </c>
+      <c t="s" r="G270">
         <v>481</v>
-      </c>
-      <c t="s" r="G270">
-        <v>482</v>
       </c>
     </row>
     <row r="271">
@@ -5540,16 +5537,16 @@
         <v>30</v>
       </c>
       <c t="s" r="F271">
+        <v>482</v>
+      </c>
+      <c t="s" s="9" r="G271">
         <v>483</v>
       </c>
-      <c t="s" s="9" r="G271">
+      <c t="s" r="H271">
         <v>484</v>
       </c>
-      <c t="s" r="H271">
+      <c t="s" s="9" r="I271">
         <v>485</v>
-      </c>
-      <c t="s" s="9" r="I271">
-        <v>486</v>
       </c>
     </row>
     <row r="272">
@@ -5558,10 +5555,10 @@
         <v>30</v>
       </c>
       <c t="s" r="F272">
+        <v>486</v>
+      </c>
+      <c t="s" r="G272">
         <v>487</v>
-      </c>
-      <c t="s" r="G272">
-        <v>488</v>
       </c>
     </row>
     <row r="273">
@@ -5570,10 +5567,10 @@
         <v>30</v>
       </c>
       <c t="s" r="F273">
+        <v>488</v>
+      </c>
+      <c t="s" r="G273">
         <v>489</v>
-      </c>
-      <c t="s" r="G273">
-        <v>490</v>
       </c>
     </row>
     <row r="274">
@@ -5582,10 +5579,10 @@
         <v>30</v>
       </c>
       <c t="s" r="F274">
+        <v>490</v>
+      </c>
+      <c t="s" r="G274">
         <v>491</v>
-      </c>
-      <c t="s" r="G274">
-        <v>492</v>
       </c>
     </row>
     <row r="275">
@@ -5594,10 +5591,10 @@
         <v>30</v>
       </c>
       <c t="s" r="F275">
+        <v>492</v>
+      </c>
+      <c t="s" r="G275">
         <v>493</v>
-      </c>
-      <c t="s" r="G275">
-        <v>494</v>
       </c>
     </row>
     <row r="276">
@@ -5612,33 +5609,33 @@
         <v>30</v>
       </c>
       <c t="s" r="F277">
+        <v>471</v>
+      </c>
+      <c t="s" r="G277">
         <v>472</v>
       </c>
-      <c t="s" r="G277">
-        <v>473</v>
-      </c>
       <c t="s" r="H277">
+        <v>494</v>
+      </c>
+      <c t="s" r="I277">
         <v>495</v>
-      </c>
-      <c t="s" r="I277">
-        <v>496</v>
       </c>
     </row>
     <row r="278">
       <c s="12" r="A278"/>
       <c t="s" r="B278">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="279">
       <c s="12" r="A279"/>
       <c t="s" s="8" r="B279">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="280">
       <c t="s" s="12" r="A280">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c t="s" r="B280">
         <v>29</v>
@@ -5650,10 +5647,10 @@
     <row r="281">
       <c s="12" r="A281"/>
       <c t="s" r="F281">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c t="s" r="G281">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="282">
@@ -5664,7 +5661,7 @@
     </row>
     <row r="283">
       <c t="s" s="12" r="A283">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c t="s" r="B283">
         <v>29</v>
@@ -5676,10 +5673,10 @@
     <row r="284">
       <c s="12" r="A284"/>
       <c t="s" r="F284">
+        <v>464</v>
+      </c>
+      <c t="s" r="G284">
         <v>465</v>
-      </c>
-      <c t="s" r="G284">
-        <v>466</v>
       </c>
     </row>
     <row r="285">
@@ -5700,10 +5697,10 @@
         <v>30</v>
       </c>
       <c t="s" r="F287">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c t="s" r="G287">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="288">
@@ -5712,10 +5709,10 @@
         <v>30</v>
       </c>
       <c t="s" r="F288">
+        <v>480</v>
+      </c>
+      <c t="s" r="G288">
         <v>481</v>
-      </c>
-      <c t="s" r="G288">
-        <v>482</v>
       </c>
     </row>
     <row r="289">
@@ -5724,10 +5721,10 @@
         <v>30</v>
       </c>
       <c t="s" r="F289">
+        <v>499</v>
+      </c>
+      <c t="s" r="G289">
         <v>500</v>
-      </c>
-      <c t="s" r="G289">
-        <v>501</v>
       </c>
     </row>
     <row r="290">
@@ -5736,16 +5733,16 @@
         <v>30</v>
       </c>
       <c t="s" r="F290">
+        <v>501</v>
+      </c>
+      <c t="s" r="G290">
+        <v>483</v>
+      </c>
+      <c t="s" r="H290">
         <v>502</v>
       </c>
-      <c t="s" r="G290">
-        <v>484</v>
-      </c>
-      <c t="s" r="H290">
+      <c t="s" r="I290">
         <v>503</v>
-      </c>
-      <c t="s" r="I290">
-        <v>504</v>
       </c>
     </row>
     <row r="291">
@@ -5754,10 +5751,10 @@
         <v>30</v>
       </c>
       <c t="s" r="F291">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c t="s" r="G291">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="292">
@@ -5766,10 +5763,10 @@
         <v>30</v>
       </c>
       <c t="s" r="F292">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c t="s" r="G292">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="293">
@@ -5778,10 +5775,10 @@
         <v>30</v>
       </c>
       <c t="s" r="F293">
+        <v>490</v>
+      </c>
+      <c t="s" r="G293">
         <v>491</v>
-      </c>
-      <c t="s" r="G293">
-        <v>492</v>
       </c>
     </row>
     <row r="294">
@@ -5790,10 +5787,10 @@
         <v>30</v>
       </c>
       <c t="s" r="F294">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c t="s" r="G294">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="295">
@@ -5802,16 +5799,16 @@
         <v>30</v>
       </c>
       <c t="s" r="F295">
+        <v>471</v>
+      </c>
+      <c t="s" r="G295">
         <v>472</v>
       </c>
-      <c t="s" r="G295">
-        <v>473</v>
-      </c>
       <c t="s" r="H295">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c t="s" r="I295">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="296">
@@ -5823,13 +5820,13 @@
     <row r="297">
       <c s="12" r="A297"/>
       <c t="s" r="B297">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="298">
       <c s="12" r="A298"/>
       <c t="s" s="8" r="B298">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="299">
@@ -5844,24 +5841,24 @@
         <v>30</v>
       </c>
       <c t="s" r="F300">
+        <v>453</v>
+      </c>
+      <c t="s" r="G300">
         <v>454</v>
-      </c>
-      <c t="s" r="G300">
-        <v>455</v>
       </c>
     </row>
     <row r="301">
       <c t="s" s="12" r="A301">
+        <v>507</v>
+      </c>
+      <c t="s" r="B301">
+        <v>30</v>
+      </c>
+      <c t="s" r="C301">
         <v>508</v>
       </c>
-      <c t="s" r="B301">
-        <v>30</v>
-      </c>
-      <c t="s" r="C301">
+      <c t="s" r="F301">
         <v>509</v>
-      </c>
-      <c t="s" r="F301">
-        <v>510</v>
       </c>
       <c s="9" r="G301"/>
     </row>
@@ -5883,10 +5880,10 @@
         <v>30</v>
       </c>
       <c t="s" r="F304">
+        <v>464</v>
+      </c>
+      <c t="s" r="G304">
         <v>465</v>
-      </c>
-      <c t="s" r="G304">
-        <v>466</v>
       </c>
     </row>
     <row r="305">
@@ -5895,7 +5892,7 @@
         <v>30</v>
       </c>
       <c t="s" r="F305">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c s="9" r="G305"/>
     </row>
@@ -5905,10 +5902,10 @@
         <v>30</v>
       </c>
       <c t="s" r="C306">
+        <v>510</v>
+      </c>
+      <c t="s" r="F306">
         <v>511</v>
-      </c>
-      <c t="s" r="F306">
-        <v>512</v>
       </c>
       <c s="9" r="G306"/>
     </row>
@@ -5930,10 +5927,10 @@
         <v>30</v>
       </c>
       <c t="s" r="F309">
+        <v>478</v>
+      </c>
+      <c t="s" r="G309">
         <v>479</v>
-      </c>
-      <c t="s" r="G309">
-        <v>480</v>
       </c>
     </row>
     <row r="310">
@@ -5942,10 +5939,10 @@
         <v>30</v>
       </c>
       <c t="s" r="F310">
+        <v>512</v>
+      </c>
+      <c t="s" r="G310">
         <v>513</v>
-      </c>
-      <c t="s" r="G310">
-        <v>514</v>
       </c>
     </row>
     <row r="311">
@@ -5954,16 +5951,16 @@
         <v>30</v>
       </c>
       <c t="s" r="F311">
+        <v>471</v>
+      </c>
+      <c t="s" r="G311">
         <v>472</v>
       </c>
-      <c t="s" r="G311">
-        <v>473</v>
-      </c>
       <c t="s" r="H311">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c t="s" r="I311">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="312">
@@ -5975,7 +5972,7 @@
     <row r="313">
       <c s="12" r="A313"/>
       <c t="s" s="9" r="B313">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="314">
@@ -6001,47 +5998,47 @@
         <v>3</v>
       </c>
       <c t="s" r="B1">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="2">
       <c t="s" r="A2">
+        <v>517</v>
+      </c>
+      <c t="s" r="B2">
         <v>518</v>
-      </c>
-      <c t="s" r="B2">
-        <v>519</v>
       </c>
     </row>
     <row r="3">
       <c t="s" r="A3">
+        <v>519</v>
+      </c>
+      <c t="s" r="B3">
         <v>520</v>
-      </c>
-      <c t="s" r="B3">
-        <v>521</v>
       </c>
     </row>
     <row r="4">
       <c t="s" r="A4">
+        <v>521</v>
+      </c>
+      <c t="s" r="B4">
         <v>522</v>
-      </c>
-      <c t="s" r="B4">
-        <v>523</v>
       </c>
     </row>
     <row r="5">
       <c t="s" r="A5">
+        <v>523</v>
+      </c>
+      <c t="s" r="B5">
         <v>524</v>
-      </c>
-      <c t="s" r="B5">
-        <v>525</v>
       </c>
     </row>
     <row r="6">
       <c t="s" r="A6">
+        <v>525</v>
+      </c>
+      <c t="s" r="B6">
         <v>526</v>
-      </c>
-      <c t="s" r="B6">
-        <v>527</v>
       </c>
     </row>
   </sheetData>
@@ -6057,7 +6054,7 @@
   <sheetData>
     <row r="1">
       <c t="s" s="2" r="A1">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c t="s" s="2" r="B1">
         <v>3</v>
@@ -6069,35 +6066,35 @@
         <v>6</v>
       </c>
       <c t="s" r="E1">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="2" r="A2">
+        <v>529</v>
+      </c>
+      <c t="s" s="2" r="B2">
         <v>530</v>
       </c>
-      <c t="s" s="2" r="B2">
+      <c t="s" s="2" r="C2">
         <v>531</v>
       </c>
-      <c t="s" s="2" r="C2">
+      <c t="s" r="D2">
         <v>532</v>
-      </c>
-      <c t="s" r="D2">
-        <v>533</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="2" r="A3">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c t="s" s="2" r="B3">
+        <v>533</v>
+      </c>
+      <c t="s" s="2" r="C3">
         <v>534</v>
       </c>
-      <c t="s" s="2" r="C3">
+      <c t="s" r="D3">
         <v>535</v>
-      </c>
-      <c t="s" r="D3">
-        <v>536</v>
       </c>
     </row>
     <row r="4">
@@ -6107,30 +6104,30 @@
     </row>
     <row r="5">
       <c t="s" s="2" r="A5">
+        <v>536</v>
+      </c>
+      <c t="s" s="2" r="B5">
+        <v>536</v>
+      </c>
+      <c t="s" s="2" r="C5">
         <v>537</v>
       </c>
-      <c t="s" s="2" r="B5">
-        <v>537</v>
-      </c>
-      <c t="s" s="2" r="C5">
+      <c t="s" r="D5">
         <v>538</v>
-      </c>
-      <c t="s" r="D5">
-        <v>539</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="2" r="A6">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c t="s" s="2" r="B6">
+        <v>539</v>
+      </c>
+      <c t="s" s="2" r="C6">
         <v>540</v>
       </c>
-      <c t="s" s="2" r="C6">
+      <c t="s" r="D6">
         <v>541</v>
-      </c>
-      <c t="s" r="D6">
-        <v>542</v>
       </c>
     </row>
     <row r="7">
@@ -6140,30 +6137,30 @@
     </row>
     <row r="8">
       <c t="s" s="2" r="A8">
+        <v>542</v>
+      </c>
+      <c t="s" s="2" r="B8">
+        <v>542</v>
+      </c>
+      <c t="s" s="2" r="C8">
         <v>543</v>
       </c>
-      <c t="s" s="2" r="B8">
-        <v>543</v>
-      </c>
-      <c t="s" s="2" r="C8">
+      <c t="s" r="D8">
         <v>544</v>
-      </c>
-      <c t="s" r="D8">
-        <v>545</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="2" r="A9">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c t="s" s="2" r="B9">
+        <v>545</v>
+      </c>
+      <c t="s" s="2" r="C9">
         <v>546</v>
       </c>
-      <c t="s" s="2" r="C9">
+      <c t="s" r="D9">
         <v>547</v>
-      </c>
-      <c t="s" r="D9">
-        <v>548</v>
       </c>
     </row>
     <row r="10">
@@ -6173,30 +6170,30 @@
     </row>
     <row r="11">
       <c t="s" s="2" r="A11">
+        <v>548</v>
+      </c>
+      <c t="s" s="2" r="B11">
         <v>549</v>
       </c>
-      <c t="s" s="2" r="B11">
+      <c t="s" s="2" r="C11">
         <v>550</v>
       </c>
-      <c t="s" s="2" r="C11">
+      <c t="s" r="D11">
         <v>551</v>
-      </c>
-      <c t="s" r="D11">
-        <v>552</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="2" r="A12">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c t="s" s="2" r="B12">
+        <v>552</v>
+      </c>
+      <c t="s" s="2" r="C12">
         <v>553</v>
       </c>
-      <c t="s" s="2" r="C12">
+      <c t="s" r="D12">
         <v>554</v>
-      </c>
-      <c t="s" r="D12">
-        <v>555</v>
       </c>
     </row>
     <row r="13">
@@ -6210,86 +6207,86 @@
     </row>
     <row r="15">
       <c t="s" s="2" r="A15">
+        <v>555</v>
+      </c>
+      <c t="s" s="2" r="B15">
         <v>556</v>
       </c>
-      <c t="s" s="2" r="B15">
+      <c t="s" r="C15">
         <v>557</v>
       </c>
-      <c t="s" r="C15">
+      <c t="s" r="D15">
         <v>558</v>
-      </c>
-      <c t="s" r="D15">
-        <v>559</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="2" r="A16">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c t="s" s="2" r="B16">
+        <v>559</v>
+      </c>
+      <c t="s" r="C16">
         <v>560</v>
       </c>
-      <c t="s" r="C16">
+      <c t="s" r="D16">
         <v>561</v>
-      </c>
-      <c t="s" r="D16">
-        <v>562</v>
       </c>
     </row>
     <row r="17">
       <c t="s" s="2" r="A17">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c t="s" r="B17">
+        <v>562</v>
+      </c>
+      <c t="s" r="C17">
         <v>563</v>
       </c>
-      <c t="s" r="C17">
+      <c t="s" r="D17">
         <v>564</v>
-      </c>
-      <c t="s" r="D17">
-        <v>565</v>
       </c>
     </row>
     <row r="20">
       <c t="s" r="A20">
+        <v>565</v>
+      </c>
+      <c t="s" r="B20">
         <v>566</v>
       </c>
-      <c t="s" r="B20">
+      <c t="s" r="C20">
         <v>567</v>
       </c>
-      <c t="s" r="C20">
+      <c t="s" r="D20">
         <v>568</v>
-      </c>
-      <c t="s" r="D20">
-        <v>569</v>
       </c>
     </row>
     <row r="21">
       <c t="s" r="A21">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c t="s" r="B21">
+        <v>569</v>
+      </c>
+      <c t="s" r="C21">
         <v>570</v>
       </c>
-      <c t="s" r="C21">
+      <c t="s" r="D21">
         <v>571</v>
-      </c>
-      <c t="s" r="D21">
-        <v>572</v>
       </c>
     </row>
     <row r="22">
       <c t="s" r="A22">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c t="s" r="B22">
+        <v>572</v>
+      </c>
+      <c t="s" r="C22">
         <v>573</v>
       </c>
-      <c t="s" r="C22">
+      <c t="s" r="D22">
         <v>574</v>
-      </c>
-      <c t="s" r="D22">
-        <v>575</v>
       </c>
     </row>
     <row r="24">
@@ -6299,58 +6296,58 @@
     </row>
     <row r="25">
       <c t="s" s="2" r="A25">
+        <v>575</v>
+      </c>
+      <c t="s" s="2" r="B25">
+        <v>566</v>
+      </c>
+      <c t="s" s="2" r="C25">
         <v>576</v>
       </c>
-      <c t="s" s="2" r="B25">
-        <v>567</v>
-      </c>
-      <c t="s" s="2" r="C25">
+      <c t="s" r="D25">
         <v>577</v>
-      </c>
-      <c t="s" r="D25">
-        <v>578</v>
       </c>
     </row>
     <row r="26">
       <c t="s" s="2" r="A26">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c t="s" r="B26">
+        <v>578</v>
+      </c>
+      <c t="s" r="C26">
         <v>579</v>
       </c>
-      <c t="s" r="C26">
+      <c t="s" r="D26">
         <v>580</v>
-      </c>
-      <c t="s" r="D26">
-        <v>581</v>
       </c>
     </row>
     <row r="27">
       <c t="s" s="2" r="A27">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c t="s" r="B27">
+        <v>581</v>
+      </c>
+      <c t="s" r="C27">
         <v>582</v>
       </c>
-      <c t="s" r="C27">
+      <c t="s" r="D27">
         <v>583</v>
-      </c>
-      <c t="s" r="D27">
-        <v>584</v>
       </c>
     </row>
     <row r="30">
       <c t="s" r="A30">
+        <v>584</v>
+      </c>
+      <c t="s" r="B30">
         <v>585</v>
       </c>
-      <c t="s" r="B30">
+      <c t="s" s="3" r="C30">
         <v>586</v>
       </c>
-      <c t="s" s="3" r="C30">
+      <c t="s" r="D30">
         <v>587</v>
-      </c>
-      <c t="s" r="D30">
-        <v>588</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -6358,16 +6355,16 @@
     </row>
     <row r="31">
       <c t="s" r="A31">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c t="s" r="B31">
+        <v>588</v>
+      </c>
+      <c t="s" s="3" r="C31">
         <v>589</v>
       </c>
-      <c t="s" s="3" r="C31">
+      <c t="s" r="D31">
         <v>590</v>
-      </c>
-      <c t="s" r="D31">
-        <v>591</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -6375,16 +6372,16 @@
     </row>
     <row r="32">
       <c t="s" r="A32">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c t="s" r="B32">
+        <v>591</v>
+      </c>
+      <c t="s" s="3" r="C32">
         <v>592</v>
       </c>
-      <c t="s" s="3" r="C32">
+      <c t="s" r="D32">
         <v>593</v>
-      </c>
-      <c t="s" r="D32">
-        <v>594</v>
       </c>
       <c r="E32">
         <v>1.5</v>
@@ -6392,16 +6389,16 @@
     </row>
     <row r="33">
       <c t="s" r="A33">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c t="s" r="B33">
+        <v>594</v>
+      </c>
+      <c t="s" s="3" r="C33">
         <v>595</v>
       </c>
-      <c t="s" s="3" r="C33">
+      <c t="s" r="D33">
         <v>596</v>
-      </c>
-      <c t="s" r="D33">
-        <v>597</v>
       </c>
       <c r="E33">
         <v>1.5</v>
@@ -6409,366 +6406,366 @@
     </row>
     <row r="35">
       <c t="s" r="A35">
+        <v>597</v>
+      </c>
+      <c t="s" r="B35">
         <v>598</v>
       </c>
-      <c t="s" r="B35">
+      <c t="s" r="C35">
         <v>599</v>
       </c>
-      <c t="s" r="C35">
+      <c t="s" r="D35">
         <v>600</v>
-      </c>
-      <c t="s" r="D35">
-        <v>601</v>
       </c>
     </row>
     <row r="36">
       <c t="s" r="A36">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c t="s" r="B36">
+        <v>601</v>
+      </c>
+      <c t="s" r="C36">
         <v>602</v>
       </c>
-      <c t="s" r="C36">
+      <c t="s" r="D36">
         <v>603</v>
-      </c>
-      <c t="s" r="D36">
-        <v>604</v>
       </c>
     </row>
     <row r="37">
       <c t="s" r="A37">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c t="s" r="B37">
+        <v>604</v>
+      </c>
+      <c t="s" r="C37">
         <v>605</v>
       </c>
-      <c t="s" r="C37">
+      <c t="s" r="D37">
         <v>606</v>
-      </c>
-      <c t="s" r="D37">
-        <v>607</v>
       </c>
     </row>
     <row r="38">
       <c t="s" r="A38">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c t="s" s="2" r="B38">
+        <v>607</v>
+      </c>
+      <c t="s" s="2" r="C38">
         <v>608</v>
       </c>
-      <c t="s" s="2" r="C38">
+      <c t="s" r="D38">
         <v>609</v>
-      </c>
-      <c t="s" r="D38">
-        <v>610</v>
       </c>
     </row>
     <row r="39">
       <c t="s" r="A39">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c t="s" r="B39">
+        <v>610</v>
+      </c>
+      <c t="s" s="2" r="C39">
         <v>611</v>
       </c>
-      <c t="s" s="2" r="C39">
+      <c t="s" r="D39">
         <v>612</v>
-      </c>
-      <c t="s" r="D39">
-        <v>613</v>
       </c>
     </row>
     <row r="40">
       <c t="s" r="A40">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c t="s" r="B40">
+        <v>613</v>
+      </c>
+      <c t="s" r="C40">
         <v>614</v>
       </c>
-      <c t="s" r="C40">
+      <c t="s" r="D40">
         <v>615</v>
-      </c>
-      <c t="s" r="D40">
-        <v>616</v>
       </c>
     </row>
     <row r="41">
       <c t="s" r="A41">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c t="s" r="B41">
+        <v>616</v>
+      </c>
+      <c t="s" r="C41">
         <v>617</v>
       </c>
-      <c t="s" r="C41">
+      <c t="s" r="D41">
         <v>618</v>
-      </c>
-      <c t="s" r="D41">
-        <v>619</v>
       </c>
     </row>
     <row r="42">
       <c t="s" r="A42">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c t="s" r="B42">
+        <v>619</v>
+      </c>
+      <c t="s" r="C42">
         <v>620</v>
       </c>
-      <c t="s" r="C42">
+      <c t="s" r="D42">
         <v>621</v>
-      </c>
-      <c t="s" r="D42">
-        <v>622</v>
       </c>
     </row>
     <row r="43">
       <c t="s" r="A43">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c t="s" r="B43">
+        <v>622</v>
+      </c>
+      <c t="s" r="C43">
         <v>623</v>
       </c>
-      <c t="s" r="C43">
+      <c t="s" r="D43">
         <v>624</v>
-      </c>
-      <c t="s" r="D43">
-        <v>625</v>
       </c>
     </row>
     <row r="44">
       <c t="s" r="A44">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c t="s" r="B44">
+        <v>625</v>
+      </c>
+      <c t="s" r="C44">
         <v>626</v>
       </c>
-      <c t="s" r="C44">
+      <c t="s" r="D44">
         <v>627</v>
-      </c>
-      <c t="s" r="D44">
-        <v>628</v>
       </c>
     </row>
     <row r="45">
       <c t="s" r="A45">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c t="s" r="B45">
+        <v>628</v>
+      </c>
+      <c t="s" r="C45">
         <v>629</v>
       </c>
-      <c t="s" r="C45">
+      <c t="s" r="D45">
         <v>630</v>
-      </c>
-      <c t="s" r="D45">
-        <v>631</v>
       </c>
     </row>
     <row r="48">
       <c t="s" r="A48">
+        <v>631</v>
+      </c>
+      <c t="s" r="B48">
         <v>632</v>
       </c>
-      <c t="s" r="B48">
+      <c t="s" r="C48">
         <v>633</v>
       </c>
-      <c t="s" r="C48">
+      <c t="s" r="D48">
         <v>634</v>
-      </c>
-      <c t="s" r="D48">
-        <v>635</v>
       </c>
     </row>
     <row r="49">
       <c t="s" r="A49">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c t="s" r="B49">
+        <v>635</v>
+      </c>
+      <c t="s" r="C49">
         <v>636</v>
       </c>
-      <c t="s" r="C49">
+      <c t="s" r="D49">
         <v>637</v>
-      </c>
-      <c t="s" r="D49">
-        <v>638</v>
       </c>
     </row>
     <row r="50">
       <c t="s" r="A50">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c t="s" r="B50">
+        <v>638</v>
+      </c>
+      <c t="s" r="C50">
         <v>639</v>
       </c>
-      <c t="s" r="C50">
+      <c t="s" r="D50">
         <v>640</v>
-      </c>
-      <c t="s" r="D50">
-        <v>641</v>
       </c>
     </row>
     <row r="51">
       <c t="s" r="A51">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c t="s" r="B51">
+        <v>641</v>
+      </c>
+      <c t="s" r="C51">
         <v>642</v>
       </c>
-      <c t="s" r="C51">
+      <c t="s" r="D51">
         <v>643</v>
-      </c>
-      <c t="s" r="D51">
-        <v>644</v>
       </c>
     </row>
     <row r="54">
       <c t="s" r="A54">
+        <v>644</v>
+      </c>
+      <c t="s" r="B54">
         <v>645</v>
       </c>
-      <c t="s" r="B54">
+      <c t="s" r="C54">
         <v>646</v>
       </c>
-      <c t="s" r="C54">
+      <c t="s" r="D54">
         <v>647</v>
-      </c>
-      <c t="s" r="D54">
-        <v>648</v>
       </c>
     </row>
     <row r="55">
       <c t="s" r="A55">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c t="s" r="B55">
+        <v>648</v>
+      </c>
+      <c t="s" r="C55">
         <v>649</v>
       </c>
-      <c t="s" r="C55">
+      <c t="s" r="D55">
         <v>650</v>
-      </c>
-      <c t="s" r="D55">
-        <v>651</v>
       </c>
     </row>
     <row r="58">
       <c t="s" r="A58">
+        <v>651</v>
+      </c>
+      <c t="s" r="B58">
         <v>652</v>
       </c>
-      <c t="s" r="B58">
+      <c t="s" r="C58">
         <v>653</v>
       </c>
-      <c t="s" r="C58">
+      <c t="s" r="D58">
         <v>654</v>
-      </c>
-      <c t="s" r="D58">
-        <v>655</v>
       </c>
     </row>
     <row r="59">
       <c t="s" r="A59">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c t="s" r="B59">
+        <v>655</v>
+      </c>
+      <c t="s" r="C59">
         <v>656</v>
       </c>
-      <c t="s" r="C59">
-        <v>657</v>
-      </c>
       <c t="s" r="D59">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="60">
       <c t="s" r="A60">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c t="s" r="B60">
+        <v>657</v>
+      </c>
+      <c t="s" r="C60">
         <v>658</v>
       </c>
-      <c t="s" r="C60">
+      <c t="s" r="D60">
         <v>659</v>
-      </c>
-      <c t="s" r="D60">
-        <v>660</v>
       </c>
     </row>
     <row r="61">
       <c t="s" r="A61">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c t="s" r="B61">
+        <v>660</v>
+      </c>
+      <c t="s" r="C61">
         <v>661</v>
       </c>
-      <c t="s" r="C61">
+      <c t="s" r="D61">
         <v>662</v>
-      </c>
-      <c t="s" r="D61">
-        <v>663</v>
       </c>
     </row>
     <row r="63">
       <c t="s" r="A63">
+        <v>663</v>
+      </c>
+      <c t="s" r="B63">
+        <v>566</v>
+      </c>
+      <c t="s" r="C63">
+        <v>566</v>
+      </c>
+      <c t="s" r="D63">
         <v>664</v>
-      </c>
-      <c t="s" r="B63">
-        <v>567</v>
-      </c>
-      <c t="s" r="C63">
-        <v>567</v>
-      </c>
-      <c t="s" r="D63">
-        <v>665</v>
       </c>
     </row>
     <row r="64">
       <c t="s" r="A64">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c t="s" r="B64">
+        <v>665</v>
+      </c>
+      <c t="s" r="C64">
+        <v>665</v>
+      </c>
+      <c t="s" r="D64">
         <v>666</v>
-      </c>
-      <c t="s" r="C64">
-        <v>666</v>
-      </c>
-      <c t="s" r="D64">
-        <v>667</v>
       </c>
     </row>
     <row r="65">
       <c t="s" r="A65">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c t="s" r="B65">
+        <v>667</v>
+      </c>
+      <c t="s" r="C65">
+        <v>667</v>
+      </c>
+      <c t="s" r="D65">
         <v>668</v>
-      </c>
-      <c t="s" r="C65">
-        <v>668</v>
-      </c>
-      <c t="s" r="D65">
-        <v>669</v>
       </c>
     </row>
     <row r="67">
       <c t="s" r="A67">
+        <v>669</v>
+      </c>
+      <c t="s" r="B67">
         <v>670</v>
       </c>
-      <c t="s" r="B67">
+      <c t="s" r="C67">
         <v>671</v>
       </c>
-      <c t="s" r="C67">
+      <c t="s" r="D67">
         <v>672</v>
-      </c>
-      <c t="s" r="D67">
-        <v>673</v>
       </c>
     </row>
     <row r="68">
       <c t="s" r="A68">
+        <v>673</v>
+      </c>
+      <c t="s" r="B68">
         <v>674</v>
       </c>
-      <c t="s" r="B68">
+      <c t="s" r="C68">
         <v>675</v>
       </c>
-      <c t="s" r="C68">
+      <c t="s" r="D68">
         <v>676</v>
-      </c>
-      <c t="s" r="D68">
-        <v>677</v>
       </c>
     </row>
     <row r="70">
@@ -6776,13 +6773,13 @@
         <v>100</v>
       </c>
       <c t="s" r="B70">
+        <v>677</v>
+      </c>
+      <c t="s" r="C70">
         <v>678</v>
       </c>
-      <c t="s" r="C70">
+      <c t="s" r="D70">
         <v>679</v>
-      </c>
-      <c t="s" r="D70">
-        <v>680</v>
       </c>
     </row>
     <row r="71">
@@ -6790,13 +6787,13 @@
         <v>100</v>
       </c>
       <c t="s" r="B71">
+        <v>680</v>
+      </c>
+      <c t="s" r="C71">
         <v>681</v>
       </c>
-      <c t="s" r="C71">
+      <c t="s" r="D71">
         <v>682</v>
-      </c>
-      <c t="s" r="D71">
-        <v>683</v>
       </c>
     </row>
   </sheetData>
@@ -6812,29 +6809,29 @@
   <sheetData>
     <row r="1">
       <c t="s" s="2" r="A1">
+        <v>683</v>
+      </c>
+      <c t="s" s="2" r="B1">
         <v>684</v>
       </c>
-      <c t="s" s="2" r="B1">
+      <c t="s" s="2" r="C1">
         <v>685</v>
-      </c>
-      <c t="s" s="2" r="C1">
-        <v>686</v>
       </c>
       <c s="2" r="D1"/>
     </row>
     <row r="2">
       <c t="s" s="2" r="A2">
+        <v>686</v>
+      </c>
+      <c t="s" s="2" r="B2">
         <v>687</v>
-      </c>
-      <c t="s" s="2" r="B2">
-        <v>688</v>
       </c>
       <c s="2" r="C2"/>
       <c s="2" r="D2"/>
     </row>
     <row r="3">
       <c t="s" s="2" r="A3">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -6843,13 +6840,13 @@
     </row>
     <row r="4">
       <c t="s" r="A4">
+        <v>689</v>
+      </c>
+      <c t="s" r="B4">
         <v>690</v>
       </c>
-      <c t="s" r="B4">
+      <c t="s" r="C4">
         <v>691</v>
-      </c>
-      <c t="s" r="C4">
-        <v>692</v>
       </c>
     </row>
     <row r="6">

</xml_diff>